<commit_message>
refactor students choice importing
</commit_message>
<xml_diff>
--- a/src/test/resources/parser/students_choice.xlsx
+++ b/src/test/resources/parser/students_choice.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t xml:space="preserve">Прізвище </t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>Семестр</t>
+  </si>
+  <si>
+    <t>Маг-майнер</t>
+  </si>
+  <si>
+    <t>Назва</t>
+  </si>
+  <si>
+    <t>Комунікація у професійній діяльності (АНГЛ)</t>
+  </si>
+  <si>
+    <t>Управління діловою кар’єрою</t>
+  </si>
+  <si>
+    <t>Планування розвитку територій</t>
   </si>
 </sst>
 </file>
@@ -172,7 +187,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,8 +211,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -217,8 +234,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -230,6 +251,7 @@
     <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -242,6 +264,7 @@
     <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -516,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,9 +552,10 @@
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,13 +572,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -570,14 +600,20 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6">
-        <v>1</v>
+      <c r="F2" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
       </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -593,14 +629,20 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6">
-        <v>1</v>
+      <c r="F3" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
       </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -616,14 +658,20 @@
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6">
-        <v>1</v>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="6">
         <v>1</v>
       </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -639,11 +687,17 @@
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6">
-        <v>1</v>
+      <c r="F5" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>